<commit_message>
Bug fixes and new features
- Will now record and save new videos music in the datasets
- Attempts to automatically extract info from music files
- Better logic for classifying videos
- Option to filter on only videos that have been classified (more speedy quality pmvs)
- Option to download videos only
- General bug fixes improvements
</commit_message>
<xml_diff>
--- a/Resources/DataLists/PathListReduced.xlsx
+++ b/Resources/DataLists/PathListReduced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Main\PycharmProjects\PMV_Generator_Git\Resources\DataLists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1871AE8-28B8-4555-9853-A31A5E171F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB62F93-E783-4294-8092-C6CC207A7F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="1530" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>PathName</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>Resources/TempMusicVid/</t>
+  </si>
+  <si>
+    <t>ArtistListPath</t>
+  </si>
+  <si>
+    <t>Resources/DataLists/ArtistList.csv</t>
   </si>
 </sst>
 </file>
@@ -517,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -647,6 +653,14 @@
       </c>
       <c r="B15" s="2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>